<commit_message>
DER revisado. Acrescentadas tabelas.
</commit_message>
<xml_diff>
--- a/ProjetoBancoDados/impacta-es13-pbd-ModeloRelacionaL.xlsx
+++ b/ProjetoBancoDados/impacta-es13-pbd-ModeloRelacionaL.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -148,6 +148,24 @@
   </si>
   <si>
     <t>DDD</t>
+  </si>
+  <si>
+    <t>Separado</t>
+  </si>
+  <si>
+    <t>ID Funcinário</t>
+  </si>
+  <si>
+    <t>Conferido</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Status Pedido</t>
+  </si>
+  <si>
+    <t>ID Status</t>
   </si>
 </sst>
 </file>
@@ -610,13 +628,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>895350</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -670,13 +688,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -902,6 +920,306 @@
           <a:r>
             <a:rPr lang="pt-BR" sz="1100"/>
             <a:t>Tem</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Texto explicativo retangular 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2924175" y="6762750"/>
+          <a:ext cx="866775" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -28626"/>
+            <a:gd name="adj2" fmla="val 87592"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Atualiza</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>781051</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Texto explicativo retangular 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114801" y="6772275"/>
+          <a:ext cx="342900" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -28626"/>
+            <a:gd name="adj2" fmla="val 87592"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>É</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Texto explicativo retangular 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1990725" y="7343775"/>
+          <a:ext cx="866775" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -28626"/>
+            <a:gd name="adj2" fmla="val 87592"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Atualiza</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>561976</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>904876</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Texto explicativo retangular 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181351" y="7353300"/>
+          <a:ext cx="342900" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -28626"/>
+            <a:gd name="adj2" fmla="val 87592"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>É</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Texto explicativo retangular 16"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7820025" y="5029200"/>
+          <a:ext cx="571500" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -41613"/>
+            <a:gd name="adj2" fmla="val 87501"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100"/>
+            <a:t>Possui</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1174,10 +1492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,9 +1504,10 @@
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1431,14 +1750,20 @@
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1483,6 +1808,57 @@
       </c>
       <c r="D35" s="2" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revisão dos artefatos de banco de dados.
</commit_message>
<xml_diff>
--- a/ProjetoBancoDados/impacta-es13-pbd-ModeloRelacionaL.xlsx
+++ b/ProjetoBancoDados/impacta-es13-pbd-ModeloRelacionaL.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -150,22 +150,22 @@
     <t>DDD</t>
   </si>
   <si>
-    <t>Separado</t>
-  </si>
-  <si>
-    <t>ID Funcinário</t>
-  </si>
-  <si>
-    <t>Conferido</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>Status Pedido</t>
-  </si>
-  <si>
-    <t>ID Status</t>
+    <t>Data separado</t>
+  </si>
+  <si>
+    <t>Data conferido</t>
+  </si>
+  <si>
+    <t>Observação</t>
+  </si>
+  <si>
+    <t>Separado por (ID Funcinário)</t>
+  </si>
+  <si>
+    <t>Conferido por (ID Funcionário)</t>
   </si>
 </sst>
 </file>
@@ -928,31 +928,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1038226</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1762126</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Texto explicativo retangular 12"/>
+        <xdr:cNvPr id="18" name="Texto explicativo retangular 17"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2924175" y="6762750"/>
-          <a:ext cx="866775" cy="238125"/>
+          <a:off x="8191501" y="5000625"/>
+          <a:ext cx="723900" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -28626"/>
-            <a:gd name="adj2" fmla="val 87592"/>
+            <a:gd name="adj1" fmla="val -5249"/>
+            <a:gd name="adj2" fmla="val 101137"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -979,7 +979,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>Atualiza</a:t>
+            <a:t>Contém</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -988,31 +988,31 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>438151</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>781051</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1647825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Texto explicativo retangular 13"/>
+        <xdr:cNvPr id="19" name="Texto explicativo retangular 18"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4114801" y="6772275"/>
-          <a:ext cx="342900" cy="238125"/>
+          <a:off x="10791825" y="4991100"/>
+          <a:ext cx="733425" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -28626"/>
-            <a:gd name="adj2" fmla="val 87592"/>
+            <a:gd name="adj1" fmla="val -5249"/>
+            <a:gd name="adj2" fmla="val 101137"/>
           </a:avLst>
         </a:prstGeom>
       </xdr:spPr>
@@ -1039,187 +1039,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>É</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Texto explicativo retangular 14"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1990725" y="7343775"/>
-          <a:ext cx="866775" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -28626"/>
-            <a:gd name="adj2" fmla="val 87592"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>Atualiza</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>561976</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>904876</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Texto explicativo retangular 15"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3181351" y="7353300"/>
-          <a:ext cx="342900" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -28626"/>
-            <a:gd name="adj2" fmla="val 87592"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>É</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Texto explicativo retangular 16"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7820025" y="5029200"/>
-          <a:ext cx="571500" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -41613"/>
-            <a:gd name="adj2" fmla="val 87501"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100"/>
-            <a:t>Possui</a:t>
+            <a:t>Contém</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1492,22 +1312,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1664,7 +1486,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1687,12 +1509,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -1706,12 +1528,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1722,12 +1544,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -1738,12 +1560,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1751,7 +1573,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>7</v>
@@ -1763,15 +1585,27 @@
         <v>31</v>
       </c>
       <c r="G29" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K29" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -1808,57 +1642,6 @@
       </c>
       <c r="D35" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1878,8 +1661,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="7:10" x14ac:dyDescent="0.25">

</xml_diff>